<commit_message>
a lot of UI changes
</commit_message>
<xml_diff>
--- a/Client/assets/Csv/Building.xlsx
+++ b/Client/assets/Csv/Building.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\AnnoArk2\Client\assets\Csv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\AnnoArk2\Client\assets\Csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,13 +15,10 @@
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">工作表1!$A$1:$AA$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">工作表1!$A$1:$AB$1</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -30,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="129">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -110,10 +107,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>workshop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>sandcoll</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -396,10 +389,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>workshop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>collector</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -505,13 +494,52 @@
   </si>
   <si>
     <t>nukemiss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Money</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>producer</t>
+  </si>
+  <si>
+    <t>silicon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ch4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iron</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chopper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ship</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nuke</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>missile</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2">
     <font>
       <sz val="12"/>
@@ -831,21 +859,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB30"/>
+  <dimension ref="A1:AC30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AA2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="27" max="27" width="10.125" customWidth="1"/>
+    <col min="28" max="28" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -856,122 +884,125 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J1" t="s">
         <v>7</v>
       </c>
       <c r="K1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L1" t="s">
         <v>119</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" t="s">
         <v>60</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>61</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>62</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>63</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>64</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>65</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>66</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
+        <v>3</v>
+      </c>
+      <c r="V1" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" t="s">
+        <v>69</v>
+      </c>
+      <c r="X1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y1" t="s">
         <v>67</v>
       </c>
-      <c r="T1" t="s">
-        <v>3</v>
-      </c>
-      <c r="U1" t="s">
-        <v>4</v>
-      </c>
-      <c r="V1" t="s">
-        <v>70</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB1" t="s">
         <v>71</v>
       </c>
-      <c r="X1" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28">
+      <c r="AC1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29">
       <c r="A2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" t="s">
         <v>97</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>99</v>
-      </c>
-      <c r="F2" t="s">
-        <v>101</v>
       </c>
       <c r="G2">
         <v>10</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
+        <v>99</v>
+      </c>
+      <c r="V2">
+        <v>5</v>
+      </c>
+      <c r="Y2" t="s">
         <v>101</v>
       </c>
-      <c r="U2">
-        <v>5</v>
-      </c>
-      <c r="X2" t="s">
-        <v>103</v>
-      </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>20</v>
       </c>
-      <c r="Z2">
+      <c r="AA2">
         <v>0</v>
       </c>
-      <c r="AA2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28">
+      <c r="AB2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -983,61 +1014,67 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G3">
         <v>8</v>
       </c>
-      <c r="T3" t="s">
-        <v>76</v>
-      </c>
-      <c r="U3">
+      <c r="U3" t="s">
+        <v>75</v>
+      </c>
+      <c r="V3">
         <v>16</v>
       </c>
-      <c r="Z3">
+      <c r="AA3">
         <v>7</v>
       </c>
-      <c r="AA3" t="str">
-        <f>A3</f>
+      <c r="AB3" t="str">
+        <f t="shared" ref="AB3:AB10" si="0">A3</f>
         <v>sandcoll</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:29">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G4">
         <v>10</v>
       </c>
+      <c r="Y4" t="s">
+        <v>75</v>
+      </c>
       <c r="Z4">
+        <v>100</v>
+      </c>
+      <c r="AA4">
         <v>7</v>
       </c>
-      <c r="AA4" t="str">
-        <f>A4</f>
+      <c r="AB4" t="str">
+        <f t="shared" si="0"/>
         <v>sandhouse</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:29">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>70</v>
@@ -1049,70 +1086,76 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="F5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G5">
         <v>10</v>
       </c>
-      <c r="L5" t="s">
-        <v>75</v>
-      </c>
-      <c r="M5">
+      <c r="M5" t="s">
+        <v>74</v>
+      </c>
+      <c r="N5">
         <v>12</v>
       </c>
-      <c r="T5" t="s">
-        <v>79</v>
-      </c>
-      <c r="V5">
-        <v>1</v>
+      <c r="U5" t="s">
+        <v>78</v>
       </c>
       <c r="W5">
+        <v>1</v>
+      </c>
+      <c r="X5">
         <v>60</v>
       </c>
-      <c r="Z5">
+      <c r="AA5">
         <v>7</v>
       </c>
-      <c r="AA5" t="str">
-        <f>A5</f>
+      <c r="AB5" t="str">
+        <f t="shared" si="0"/>
         <v>siliconprod</v>
       </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:29">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6">
         <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G6">
         <v>10</v>
       </c>
+      <c r="Y6" t="s">
+        <v>121</v>
+      </c>
       <c r="Z6">
+        <v>100</v>
+      </c>
+      <c r="AA6">
         <v>7</v>
       </c>
-      <c r="AA6" t="str">
-        <f>A6</f>
+      <c r="AB6" t="str">
+        <f t="shared" si="0"/>
         <v>siliconhouse</v>
       </c>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:29">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7">
         <v>120</v>
@@ -1124,67 +1167,73 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G7">
         <v>15</v>
       </c>
       <c r="H7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I7">
         <v>5</v>
       </c>
-      <c r="T7" t="s">
-        <v>81</v>
-      </c>
-      <c r="U7">
+      <c r="U7" t="s">
+        <v>80</v>
+      </c>
+      <c r="V7">
         <v>16</v>
       </c>
-      <c r="Z7">
+      <c r="AA7">
         <v>7</v>
       </c>
-      <c r="AA7" t="str">
-        <f>A7</f>
+      <c r="AB7" t="str">
+        <f t="shared" si="0"/>
         <v>ch4coll</v>
       </c>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:29">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8">
         <v>121</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G8">
         <v>10</v>
       </c>
+      <c r="Y8" t="s">
+        <v>122</v>
+      </c>
       <c r="Z8">
+        <v>100</v>
+      </c>
+      <c r="AA8">
         <v>7</v>
       </c>
-      <c r="AA8" t="str">
-        <f>A8</f>
+      <c r="AB8" t="str">
+        <f t="shared" si="0"/>
         <v>ch4house</v>
       </c>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:29">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9">
         <v>150</v>
@@ -1196,76 +1245,82 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="F9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G9">
         <v>10</v>
       </c>
       <c r="H9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I9">
         <v>5</v>
       </c>
-      <c r="L9" t="s">
-        <v>81</v>
-      </c>
-      <c r="M9">
+      <c r="M9" t="s">
+        <v>80</v>
+      </c>
+      <c r="N9">
         <v>12</v>
       </c>
-      <c r="T9" t="s">
-        <v>80</v>
-      </c>
-      <c r="V9">
+      <c r="U9" t="s">
+        <v>79</v>
+      </c>
+      <c r="W9">
         <v>2</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <v>40</v>
       </c>
-      <c r="Z9">
+      <c r="AA9">
         <v>7</v>
       </c>
-      <c r="AA9" t="str">
-        <f>A9</f>
+      <c r="AB9" t="str">
+        <f t="shared" si="0"/>
         <v>carbonprod</v>
       </c>
     </row>
-    <row r="10" spans="1:28">
+    <row r="10" spans="1:29">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10">
         <v>151</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G10">
         <v>10</v>
       </c>
+      <c r="Y10" t="s">
+        <v>110</v>
+      </c>
       <c r="Z10">
+        <v>100</v>
+      </c>
+      <c r="AA10">
         <v>7</v>
       </c>
-      <c r="AA10" t="str">
-        <f>A10</f>
+      <c r="AB10" t="str">
+        <f t="shared" si="0"/>
         <v>carbonhouse</v>
       </c>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:29">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11">
         <v>200</v>
@@ -1277,73 +1332,79 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G11">
         <v>10</v>
       </c>
       <c r="H11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I11">
         <v>7</v>
       </c>
       <c r="J11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K11">
         <v>3</v>
       </c>
-      <c r="T11" t="s">
-        <v>77</v>
-      </c>
-      <c r="U11">
+      <c r="U11" t="s">
+        <v>76</v>
+      </c>
+      <c r="V11">
         <v>8</v>
       </c>
-      <c r="Z11">
+      <c r="AA11">
         <v>6</v>
       </c>
-      <c r="AA11" t="str">
-        <f t="shared" ref="AA11:AA18" si="0">A11</f>
+      <c r="AB11" t="str">
+        <f t="shared" ref="AB11:AB18" si="1">A11</f>
         <v>ironcoll</v>
       </c>
     </row>
-    <row r="12" spans="1:28">
+    <row r="12" spans="1:29">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12">
         <v>201</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G12">
         <v>10</v>
       </c>
+      <c r="Y12" t="s">
+        <v>123</v>
+      </c>
       <c r="Z12">
+        <v>100</v>
+      </c>
+      <c r="AA12">
         <v>6</v>
       </c>
-      <c r="AA12" t="str">
-        <f t="shared" si="0"/>
+      <c r="AB12" t="str">
+        <f t="shared" si="1"/>
         <v>ironhouse</v>
       </c>
     </row>
-    <row r="13" spans="1:28">
+    <row r="13" spans="1:29">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13">
         <v>300</v>
@@ -1355,88 +1416,94 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="F13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G13">
         <v>20</v>
       </c>
       <c r="H13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I13">
         <v>10</v>
       </c>
       <c r="J13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K13">
         <v>4</v>
       </c>
-      <c r="L13" t="s">
-        <v>79</v>
-      </c>
-      <c r="M13">
+      <c r="M13" t="s">
+        <v>78</v>
+      </c>
+      <c r="N13">
         <v>40</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
+        <v>76</v>
+      </c>
+      <c r="P13">
+        <v>10</v>
+      </c>
+      <c r="U13" t="s">
         <v>77</v>
       </c>
-      <c r="O13">
-        <v>10</v>
-      </c>
-      <c r="T13" t="s">
-        <v>78</v>
-      </c>
-      <c r="V13">
+      <c r="W13">
         <v>4</v>
       </c>
-      <c r="W13">
+      <c r="X13">
         <v>30</v>
       </c>
-      <c r="Z13">
+      <c r="AA13">
         <v>5</v>
       </c>
-      <c r="AA13" t="str">
-        <f t="shared" si="0"/>
+      <c r="AB13" t="str">
+        <f t="shared" si="1"/>
         <v>chipprod</v>
       </c>
     </row>
-    <row r="14" spans="1:28">
+    <row r="14" spans="1:29">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14">
         <v>301</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G14">
         <v>50</v>
       </c>
+      <c r="Y14" t="s">
+        <v>124</v>
+      </c>
       <c r="Z14">
+        <v>100</v>
+      </c>
+      <c r="AA14">
         <v>5</v>
       </c>
-      <c r="AA14" t="str">
-        <f t="shared" si="0"/>
+      <c r="AB14" t="str">
+        <f t="shared" si="1"/>
         <v>chiphouse</v>
       </c>
     </row>
-    <row r="15" spans="1:28">
+    <row r="15" spans="1:29">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15">
         <v>350</v>
@@ -1448,94 +1515,100 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="F15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G15">
         <v>80</v>
       </c>
       <c r="H15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I15">
         <v>20</v>
       </c>
       <c r="J15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K15">
         <v>10</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
+        <v>76</v>
+      </c>
+      <c r="N15">
+        <v>60</v>
+      </c>
+      <c r="O15" t="s">
+        <v>79</v>
+      </c>
+      <c r="P15">
+        <v>20</v>
+      </c>
+      <c r="Q15" t="s">
         <v>77</v>
       </c>
-      <c r="M15">
-        <v>60</v>
-      </c>
-      <c r="N15" t="s">
-        <v>80</v>
-      </c>
-      <c r="O15">
+      <c r="R15">
         <v>20</v>
       </c>
-      <c r="P15" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q15">
+      <c r="U15" t="s">
+        <v>82</v>
+      </c>
+      <c r="W15">
+        <v>10</v>
+      </c>
+      <c r="X15">
         <v>20</v>
       </c>
-      <c r="T15" t="s">
-        <v>83</v>
-      </c>
-      <c r="V15">
-        <v>10</v>
-      </c>
-      <c r="W15">
-        <v>20</v>
-      </c>
-      <c r="Z15">
+      <c r="AA15">
         <v>4</v>
       </c>
-      <c r="AA15" t="str">
-        <f t="shared" si="0"/>
+      <c r="AB15" t="str">
+        <f t="shared" si="1"/>
         <v>tankprod</v>
       </c>
     </row>
-    <row r="16" spans="1:28">
+    <row r="16" spans="1:29">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16">
         <v>351</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G16">
         <v>80</v>
       </c>
+      <c r="Y16" t="s">
+        <v>82</v>
+      </c>
       <c r="Z16">
+        <v>10</v>
+      </c>
+      <c r="AA16">
         <v>4</v>
       </c>
-      <c r="AA16" t="str">
-        <f t="shared" si="0"/>
+      <c r="AB16" t="str">
+        <f t="shared" si="1"/>
         <v>tankhouse</v>
       </c>
     </row>
-    <row r="17" spans="1:27">
+    <row r="17" spans="1:28">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17">
         <v>400</v>
@@ -1547,94 +1620,100 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="F17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G17">
         <v>100</v>
       </c>
       <c r="H17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I17">
         <v>30</v>
       </c>
       <c r="J17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K17">
         <v>10</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
+        <v>76</v>
+      </c>
+      <c r="N17">
+        <v>40</v>
+      </c>
+      <c r="O17" t="s">
+        <v>79</v>
+      </c>
+      <c r="P17">
+        <v>40</v>
+      </c>
+      <c r="Q17" t="s">
         <v>77</v>
       </c>
-      <c r="M17">
-        <v>40</v>
-      </c>
-      <c r="N17" t="s">
-        <v>80</v>
-      </c>
-      <c r="O17">
-        <v>40</v>
-      </c>
-      <c r="P17" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q17">
+      <c r="R17">
         <v>30</v>
       </c>
-      <c r="T17" t="s">
-        <v>84</v>
-      </c>
-      <c r="V17">
+      <c r="U17" t="s">
+        <v>83</v>
+      </c>
+      <c r="W17">
         <v>10</v>
       </c>
-      <c r="W17">
+      <c r="X17">
         <v>20</v>
       </c>
-      <c r="Z17">
+      <c r="AA17">
         <v>4</v>
       </c>
-      <c r="AA17" t="str">
-        <f t="shared" si="0"/>
+      <c r="AB17" t="str">
+        <f t="shared" si="1"/>
         <v>chopperprod</v>
       </c>
     </row>
-    <row r="18" spans="1:27">
+    <row r="18" spans="1:28">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18">
         <v>401</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G18">
         <v>120</v>
       </c>
+      <c r="Y18" t="s">
+        <v>125</v>
+      </c>
       <c r="Z18">
+        <v>10</v>
+      </c>
+      <c r="AA18">
         <v>4</v>
       </c>
-      <c r="AA18" t="str">
-        <f t="shared" si="0"/>
+      <c r="AB18" t="str">
+        <f t="shared" si="1"/>
         <v>chopperhouse</v>
       </c>
     </row>
-    <row r="19" spans="1:27">
+    <row r="19" spans="1:28">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19">
         <v>500</v>
@@ -1646,94 +1725,100 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="F19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G19">
         <v>120</v>
       </c>
       <c r="H19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I19">
         <v>40</v>
       </c>
       <c r="J19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K19">
         <v>20</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
+        <v>76</v>
+      </c>
+      <c r="N19">
+        <v>80</v>
+      </c>
+      <c r="O19" t="s">
+        <v>79</v>
+      </c>
+      <c r="P19">
+        <v>30</v>
+      </c>
+      <c r="Q19" t="s">
         <v>77</v>
       </c>
-      <c r="M19">
-        <v>80</v>
-      </c>
-      <c r="N19" t="s">
-        <v>80</v>
-      </c>
-      <c r="O19">
-        <v>30</v>
-      </c>
-      <c r="P19" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q19">
+      <c r="R19">
         <v>5</v>
       </c>
-      <c r="T19" t="s">
-        <v>85</v>
-      </c>
-      <c r="V19">
+      <c r="U19" t="s">
+        <v>84</v>
+      </c>
+      <c r="W19">
         <v>50</v>
       </c>
-      <c r="W19">
+      <c r="X19">
         <v>12</v>
       </c>
-      <c r="Z19">
+      <c r="AA19">
         <v>4</v>
       </c>
-      <c r="AA19" t="str">
+      <c r="AB19" t="str">
         <f>A19</f>
         <v>shipprod</v>
       </c>
     </row>
-    <row r="20" spans="1:27">
+    <row r="20" spans="1:28">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20">
         <v>501</v>
       </c>
       <c r="C20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
         <v>52</v>
       </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>53</v>
-      </c>
       <c r="F20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G20">
         <v>120</v>
       </c>
+      <c r="Y20" t="s">
+        <v>126</v>
+      </c>
       <c r="Z20">
+        <v>10</v>
+      </c>
+      <c r="AA20">
         <v>4</v>
       </c>
-      <c r="AA20" t="str">
+      <c r="AB20" t="str">
         <f>A20</f>
         <v>shiphouse</v>
       </c>
     </row>
-    <row r="21" spans="1:27">
+    <row r="21" spans="1:28">
       <c r="A21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B21">
         <v>9000</v>
@@ -1745,91 +1830,97 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G21">
         <v>200</v>
       </c>
       <c r="H21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I21">
         <v>100</v>
       </c>
       <c r="J21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K21">
         <v>80</v>
       </c>
-      <c r="T21" t="s">
-        <v>86</v>
-      </c>
-      <c r="U21">
-        <v>1</v>
-      </c>
-      <c r="Z21">
+      <c r="L21">
+        <v>0.02</v>
+      </c>
+      <c r="U21" t="s">
+        <v>85</v>
+      </c>
+      <c r="V21">
+        <v>1.6670000000000001E-2</v>
+      </c>
+      <c r="AA21">
         <v>3</v>
       </c>
-      <c r="AA21" t="str">
+      <c r="AB21" t="str">
         <f>A21</f>
         <v>deutercoll</v>
       </c>
     </row>
-    <row r="22" spans="1:27">
+    <row r="22" spans="1:28">
       <c r="A22" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B22">
         <v>9001</v>
       </c>
       <c r="C22" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F22" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G22">
         <v>100</v>
       </c>
       <c r="H22" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I22">
         <v>100</v>
       </c>
       <c r="J22" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K22">
         <v>50</v>
       </c>
-      <c r="X22" t="s">
-        <v>115</v>
-      </c>
-      <c r="Y22">
+      <c r="L22">
+        <v>0.01</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z22">
         <v>20</v>
       </c>
-      <c r="Z22">
+      <c r="AA22">
         <v>3</v>
       </c>
-      <c r="AA22" t="str">
+      <c r="AB22" t="str">
         <f>A22</f>
         <v>deuterhouse</v>
       </c>
     </row>
-    <row r="23" spans="1:27">
+    <row r="23" spans="1:28">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23">
         <v>10000</v>
@@ -1841,243 +1932,262 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="F23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G23">
         <v>400</v>
       </c>
       <c r="H23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I23">
         <v>160</v>
       </c>
       <c r="J23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K23">
         <v>120</v>
       </c>
-      <c r="L23" t="s">
+      <c r="L23">
+        <v>0.1</v>
+      </c>
+      <c r="M23" t="s">
+        <v>76</v>
+      </c>
+      <c r="N23">
+        <v>15</v>
+      </c>
+      <c r="O23" t="s">
+        <v>80</v>
+      </c>
+      <c r="P23">
+        <v>100</v>
+      </c>
+      <c r="Q23" t="s">
         <v>77</v>
       </c>
-      <c r="M23">
-        <v>15</v>
-      </c>
-      <c r="N23" t="s">
+      <c r="R23">
+        <v>20</v>
+      </c>
+      <c r="S23" t="s">
         <v>81</v>
       </c>
-      <c r="O23">
-        <v>100</v>
-      </c>
-      <c r="P23" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q23">
-        <v>20</v>
-      </c>
-      <c r="R23" t="s">
-        <v>82</v>
-      </c>
-      <c r="S23">
+      <c r="T23">
         <v>50</v>
       </c>
-      <c r="T23" t="s">
-        <v>95</v>
-      </c>
-      <c r="U23">
-        <f>1/60</f>
-        <v>1.6666666666666666E-2</v>
-      </c>
-      <c r="V23">
+      <c r="U23" t="s">
+        <v>93</v>
+      </c>
+      <c r="W23">
         <v>720</v>
       </c>
-      <c r="W23">
+      <c r="X23">
         <v>2</v>
       </c>
-      <c r="Z23">
+      <c r="AA23">
         <v>3</v>
       </c>
-      <c r="AA23" t="str">
-        <f t="shared" ref="AA23:AA27" si="1">A23</f>
+      <c r="AB23" t="str">
+        <f t="shared" ref="AB23:AB27" si="2">A23</f>
         <v>nukeprod</v>
       </c>
     </row>
-    <row r="24" spans="1:27">
+    <row r="24" spans="1:28">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24">
         <v>10001</v>
       </c>
       <c r="C24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G24">
         <v>400</v>
       </c>
+      <c r="L24">
+        <v>0.05</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>127</v>
+      </c>
       <c r="Z24">
+        <v>1</v>
+      </c>
+      <c r="AA24">
         <v>3</v>
       </c>
-      <c r="AA24" t="str">
-        <f t="shared" si="1"/>
+      <c r="AB24" t="str">
+        <f t="shared" si="2"/>
         <v>nukehouse</v>
       </c>
     </row>
-    <row r="25" spans="1:27">
+    <row r="25" spans="1:28">
       <c r="A25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B25">
         <v>11000</v>
       </c>
       <c r="C25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="F25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G25">
         <v>400</v>
       </c>
       <c r="H25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I25">
         <v>160</v>
       </c>
       <c r="J25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K25">
         <v>120</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L25">
+        <v>0.1</v>
+      </c>
+      <c r="M25" t="s">
+        <v>76</v>
+      </c>
+      <c r="N25">
+        <v>15</v>
+      </c>
+      <c r="O25" t="s">
+        <v>80</v>
+      </c>
+      <c r="P25">
+        <v>10000</v>
+      </c>
+      <c r="Q25" t="s">
         <v>77</v>
       </c>
-      <c r="M25">
-        <v>15</v>
-      </c>
-      <c r="N25" t="s">
-        <v>81</v>
-      </c>
-      <c r="O25">
-        <v>10000</v>
-      </c>
-      <c r="P25" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q25">
+      <c r="R25">
         <v>200</v>
       </c>
-      <c r="T25" t="s">
-        <v>96</v>
-      </c>
-      <c r="U25">
-        <f>1/60</f>
-        <v>1.6666666666666666E-2</v>
-      </c>
-      <c r="V25">
+      <c r="U25" t="s">
+        <v>94</v>
+      </c>
+      <c r="W25">
         <v>720</v>
       </c>
-      <c r="W25">
+      <c r="X25">
         <v>2</v>
       </c>
-      <c r="Z25">
+      <c r="AA25">
         <v>3</v>
       </c>
-      <c r="AA25" t="str">
-        <f t="shared" si="1"/>
+      <c r="AB25" t="str">
+        <f t="shared" si="2"/>
         <v>missileprod</v>
       </c>
     </row>
-    <row r="26" spans="1:27">
+    <row r="26" spans="1:28">
       <c r="A26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B26">
         <v>11001</v>
       </c>
       <c r="C26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G26">
         <v>400</v>
       </c>
+      <c r="L26">
+        <v>0.05</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>128</v>
+      </c>
       <c r="Z26">
+        <v>1</v>
+      </c>
+      <c r="AA26">
         <v>3</v>
       </c>
-      <c r="AA26" t="str">
-        <f t="shared" si="1"/>
+      <c r="AB26" t="str">
+        <f t="shared" si="2"/>
         <v>missilehouse</v>
       </c>
     </row>
-    <row r="27" spans="1:27">
+    <row r="27" spans="1:28">
       <c r="A27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B27">
         <v>12000</v>
       </c>
       <c r="C27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>93</v>
+        <v>120</v>
       </c>
       <c r="F27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G27">
         <v>400</v>
       </c>
-      <c r="V27">
+      <c r="L27">
+        <v>0.5</v>
+      </c>
+      <c r="W27">
         <v>1440</v>
       </c>
-      <c r="W27">
-        <v>1</v>
-      </c>
-      <c r="Z27">
+      <c r="X27">
+        <v>1</v>
+      </c>
+      <c r="AA27">
         <v>3</v>
       </c>
-      <c r="AA27" t="str">
-        <f t="shared" si="1"/>
+      <c r="AB27" t="str">
+        <f t="shared" si="2"/>
         <v>nukemissprod</v>
       </c>
     </row>
-    <row r="28" spans="1:27">
+    <row r="28" spans="1:28">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28">
         <v>20000</v>
@@ -2089,82 +2199,85 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G28">
         <v>30000</v>
       </c>
       <c r="H28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I28">
         <v>20000</v>
       </c>
       <c r="J28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K28">
         <v>10000</v>
       </c>
-      <c r="X28" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y28">
-        <v>1</v>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>118</v>
       </c>
       <c r="Z28">
+        <v>1</v>
+      </c>
+      <c r="AA28">
         <v>0</v>
       </c>
-      <c r="AA28" t="str">
-        <f t="shared" ref="AA28:AA29" si="2">A28</f>
+      <c r="AB28" t="str">
+        <f t="shared" ref="AB28:AB29" si="3">A28</f>
         <v>launchsilo</v>
       </c>
     </row>
-    <row r="29" spans="1:27">
+    <row r="29" spans="1:28">
       <c r="A29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B29">
         <v>30000</v>
       </c>
       <c r="C29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G29">
         <v>10</v>
       </c>
-      <c r="X29" t="s">
-        <v>107</v>
-      </c>
-      <c r="Y29">
+      <c r="Y29" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z29">
         <v>125</v>
       </c>
-      <c r="Z29">
+      <c r="AA29">
         <v>7</v>
       </c>
-      <c r="AA29" t="str">
-        <f t="shared" si="2"/>
+      <c r="AB29" t="str">
+        <f t="shared" si="3"/>
         <v>floatmodhouse</v>
       </c>
     </row>
-    <row r="30" spans="1:27">
+    <row r="30" spans="1:28">
       <c r="A30" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" t="s">
         <v>73</v>
-      </c>
-      <c r="C30" t="s">
-        <v>74</v>
       </c>
       <c r="G30">
         <v>4</v>
@@ -2175,21 +2288,21 @@
       <c r="K30">
         <v>4</v>
       </c>
-      <c r="U30">
+      <c r="V30">
         <v>1.5</v>
       </c>
-      <c r="V30">
+      <c r="W30">
         <v>0.9</v>
       </c>
-      <c r="W30">
+      <c r="X30">
         <v>1.5</v>
       </c>
-      <c r="Y30">
+      <c r="Z30">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AA1">
+  <autoFilter ref="A1:AB1">
     <sortState ref="A2:AE18">
       <sortCondition ref="B1"/>
     </sortState>
@@ -2198,11 +2311,12 @@
     <sortCondition ref="B1"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="4">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="原料消耗速率/min/人" sqref="M1:M2 O1:O2 Q1:Q2 S1:S2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="每生产1单位需要冷却（min）" prompt="建筑刚建造完成时就进入cd状态，但此时显示为“建造中”。初次cd的时间和之后cd时间一样长。" sqref="V1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="每分钟产量" sqref="U1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="批量生产的队列容量" sqref="W1"/>
+  <dataValidations count="5">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="原料消耗速率/min/人" sqref="N1:N2 P1:P2 R1:R2 T1:T2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="每生产1单位需要冷却（min）" prompt="建筑刚建造完成时就进入cd状态，但此时显示为“建造中”。初次cd的时间和之后cd时间一样长。" sqref="W1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="每分钟产量(min)" prompt="挂机生产" sqref="V1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="批量生产的队列容量" sqref="X1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="建筑储备金" prompt="仅建造时需要支付一笔储备金，升级时不需要。_x000a_拆除时返还。" sqref="L1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
finish a lot of work
</commit_message>
<xml_diff>
--- a/Client/assets/Csv/Building.xlsx
+++ b/Client/assets/Csv/Building.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="138">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -37,10 +37,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>order</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Out0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -91,10 +87,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>直升机车间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>造船厂</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -103,10 +95,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>导弹发射井</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>sandcoll</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -215,10 +203,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>直升机机库</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>shiphouse</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -231,10 +215,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>舰艇仓库</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>warehouse</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -342,9 +322,6 @@
     <t>carbon</t>
   </si>
   <si>
-    <t>methane</t>
-  </si>
-  <si>
     <t>deuter</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -385,154 +362,213 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>氢弹导弹组装车间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>collector</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>hq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>总部</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CanBuild</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sand</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sand</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MaxLevel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>floatmodhouse</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>浮力模块仓库</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>floatmod</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>deutercoll</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>deuterhouse</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重水储存舱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>warehouse</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>carbon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iron</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>deuter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BuildMat0Cnt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BuildMat1Cnt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BuildMat2Cnt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>nukemiss</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Money</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>producer</t>
+  </si>
+  <si>
+    <t>silicon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ch4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iron</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chopper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ship</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nuke</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>missile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ch4</t>
+  </si>
+  <si>
+    <t>iron</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iron</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iron</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>炮舰仓库</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无人机车间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无人机机库</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>carbon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>silicon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>silicon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>热核导弹组装车间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>热核导弹发射井</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sand</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>missile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>nukemiss</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>hq</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>总部</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hq</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CanBuild</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sand</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sand</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MaxLevel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>floatmodhouse</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>浮力模块仓库</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>floatmod</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>deutercoll</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>deuterhouse</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>重水储存舱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>warehouse</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>carbon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>chip</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>iron</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>deuter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hq</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BuildMat0Cnt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BuildMat1Cnt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BuildMat2Cnt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nukemiss</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Money</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>producer</t>
-  </si>
-  <si>
-    <t>silicon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ch4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>iron</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>chip</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>chopper</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ship</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>nuke</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>missile</t>
+    <t>Order</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -865,7 +901,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V21" sqref="V21"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -878,117 +914,117 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>58</v>
+      </c>
+      <c r="R1" t="s">
+        <v>59</v>
+      </c>
+      <c r="S1" t="s">
+        <v>60</v>
+      </c>
+      <c r="T1" t="s">
+        <v>61</v>
+      </c>
+      <c r="U1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>116</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>117</v>
-      </c>
-      <c r="L1" t="s">
-        <v>119</v>
-      </c>
-      <c r="M1" t="s">
-        <v>59</v>
-      </c>
-      <c r="N1" t="s">
-        <v>60</v>
-      </c>
-      <c r="O1" t="s">
-        <v>61</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="V1" t="s">
+        <v>3</v>
+      </c>
+      <c r="W1" t="s">
+        <v>64</v>
+      </c>
+      <c r="X1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y1" t="s">
         <v>62</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Z1" t="s">
         <v>63</v>
       </c>
-      <c r="R1" t="s">
-        <v>64</v>
-      </c>
-      <c r="S1" t="s">
-        <v>65</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="AA1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB1" t="s">
         <v>66</v>
       </c>
-      <c r="U1" t="s">
-        <v>3</v>
-      </c>
-      <c r="V1" t="s">
-        <v>4</v>
-      </c>
-      <c r="W1" t="s">
-        <v>69</v>
-      </c>
-      <c r="X1" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>71</v>
-      </c>
       <c r="AC1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:29">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E2" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F2" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="G2">
         <v>10</v>
       </c>
       <c r="U2" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="V2">
         <v>5</v>
       </c>
       <c r="Y2" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="Z2">
         <v>20</v>
@@ -997,33 +1033,33 @@
         <v>0</v>
       </c>
       <c r="AB2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:29">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="F3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G3">
         <v>8</v>
       </c>
       <c r="U3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="V3">
         <v>16</v>
@@ -1038,28 +1074,28 @@
     </row>
     <row r="4" spans="1:29">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G4">
         <v>10</v>
       </c>
       <c r="Y4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="Z4">
         <v>100</v>
@@ -1074,34 +1110,34 @@
     </row>
     <row r="5" spans="1:29">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="F5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G5">
         <v>10</v>
       </c>
       <c r="M5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="N5">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="U5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="W5">
         <v>1</v>
@@ -1119,28 +1155,28 @@
     </row>
     <row r="6" spans="1:29">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B6">
         <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G6">
         <v>10</v>
       </c>
       <c r="Y6" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="Z6">
         <v>100</v>
@@ -1155,34 +1191,34 @@
     </row>
     <row r="7" spans="1:29">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B7">
         <v>120</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="F7" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G7">
         <v>15</v>
       </c>
       <c r="H7" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="I7">
         <v>5</v>
       </c>
       <c r="U7" t="s">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="V7">
         <v>16</v>
@@ -1197,28 +1233,34 @@
     </row>
     <row r="8" spans="1:29">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>121</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F8" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G8">
         <v>10</v>
       </c>
+      <c r="H8" t="s">
+        <v>112</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
       <c r="Y8" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="Z8">
         <v>100</v>
@@ -1233,40 +1275,40 @@
     </row>
     <row r="9" spans="1:29">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B9">
         <v>150</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
+        <v>111</v>
+      </c>
+      <c r="F9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9">
+        <v>15</v>
+      </c>
+      <c r="M9" t="s">
         <v>120</v>
       </c>
-      <c r="F9" t="s">
+      <c r="N9">
+        <v>10</v>
+      </c>
+      <c r="U9" t="s">
         <v>74</v>
-      </c>
-      <c r="G9">
-        <v>10</v>
-      </c>
-      <c r="H9" t="s">
-        <v>78</v>
-      </c>
-      <c r="I9">
-        <v>5</v>
-      </c>
-      <c r="M9" t="s">
-        <v>80</v>
-      </c>
-      <c r="N9">
-        <v>12</v>
-      </c>
-      <c r="U9" t="s">
-        <v>79</v>
       </c>
       <c r="W9">
         <v>2</v>
@@ -1284,28 +1326,28 @@
     </row>
     <row r="10" spans="1:29">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B10">
         <v>151</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G10">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="Y10" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="Z10">
         <v>100</v>
@@ -1320,40 +1362,40 @@
     </row>
     <row r="11" spans="1:29">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>200</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="F11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G11">
         <v>10</v>
       </c>
       <c r="H11" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="I11">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="J11" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="K11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="U11" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="V11">
         <v>8</v>
@@ -1368,28 +1410,28 @@
     </row>
     <row r="12" spans="1:29">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B12">
         <v>201</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G12">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="Y12" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="Z12">
         <v>100</v>
@@ -1404,52 +1446,52 @@
     </row>
     <row r="13" spans="1:29">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B13">
         <v>300</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="F13" t="s">
+        <v>103</v>
+      </c>
+      <c r="G13">
+        <v>40</v>
+      </c>
+      <c r="H13" t="s">
+        <v>73</v>
+      </c>
+      <c r="I13">
+        <v>20</v>
+      </c>
+      <c r="J13" t="s">
         <v>74</v>
       </c>
-      <c r="G13">
-        <v>20</v>
-      </c>
-      <c r="H13" t="s">
-        <v>78</v>
-      </c>
-      <c r="I13">
-        <v>10</v>
-      </c>
-      <c r="J13" t="s">
-        <v>79</v>
-      </c>
       <c r="K13">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="M13" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="N13">
         <v>40</v>
       </c>
       <c r="O13" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="P13">
         <v>10</v>
       </c>
       <c r="U13" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="W13">
         <v>4</v>
@@ -1467,28 +1509,34 @@
     </row>
     <row r="14" spans="1:29">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B14">
         <v>301</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
       <c r="G14">
-        <v>50</v>
+        <v>20</v>
+      </c>
+      <c r="H14" t="s">
+        <v>112</v>
+      </c>
+      <c r="I14">
+        <v>20</v>
       </c>
       <c r="Y14" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="Z14">
         <v>100</v>
@@ -1503,58 +1551,58 @@
     </row>
     <row r="15" spans="1:29">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>350</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="F15" t="s">
-        <v>74</v>
+        <v>122</v>
       </c>
       <c r="G15">
         <v>80</v>
       </c>
       <c r="H15" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="I15">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="J15" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="K15">
         <v>10</v>
       </c>
       <c r="M15" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="N15">
         <v>60</v>
       </c>
       <c r="O15" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="P15">
         <v>20</v>
       </c>
       <c r="Q15" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="R15">
         <v>20</v>
       </c>
       <c r="U15" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="W15">
         <v>10</v>
@@ -1572,28 +1620,34 @@
     </row>
     <row r="16" spans="1:29">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B16">
         <v>351</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F16" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
       <c r="G16">
-        <v>80</v>
+        <v>20</v>
+      </c>
+      <c r="H16" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16">
+        <v>20</v>
       </c>
       <c r="Y16" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="Z16">
         <v>10</v>
@@ -1608,58 +1662,58 @@
     </row>
     <row r="17" spans="1:28">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B17">
         <v>400</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>125</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="F17" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
       <c r="G17">
         <v>100</v>
       </c>
       <c r="H17" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="I17">
         <v>30</v>
       </c>
       <c r="J17" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="K17">
         <v>10</v>
       </c>
       <c r="M17" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="N17">
         <v>40</v>
       </c>
       <c r="O17" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="P17">
         <v>40</v>
       </c>
       <c r="Q17" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="R17">
         <v>30</v>
       </c>
       <c r="U17" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="W17">
         <v>10</v>
@@ -1677,28 +1731,34 @@
     </row>
     <row r="18" spans="1:28">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B18">
         <v>401</v>
       </c>
       <c r="C18" t="s">
+        <v>126</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
         <v>47</v>
       </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>52</v>
-      </c>
       <c r="F18" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
       <c r="G18">
         <v>120</v>
       </c>
+      <c r="H18" t="s">
+        <v>73</v>
+      </c>
+      <c r="I18">
+        <v>20</v>
+      </c>
       <c r="Y18" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="Z18">
         <v>10</v>
@@ -1713,58 +1773,58 @@
     </row>
     <row r="19" spans="1:28">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B19">
         <v>500</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="F19" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
       <c r="G19">
         <v>120</v>
       </c>
       <c r="H19" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="I19">
         <v>40</v>
       </c>
       <c r="J19" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="K19">
         <v>20</v>
       </c>
       <c r="M19" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="N19">
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="O19" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="P19">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="Q19" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="R19">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="U19" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="W19">
         <v>50</v>
@@ -1782,28 +1842,40 @@
     </row>
     <row r="20" spans="1:28">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B20">
         <v>501</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>124</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F20" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
       <c r="G20">
-        <v>120</v>
+        <v>200</v>
+      </c>
+      <c r="H20" t="s">
+        <v>112</v>
+      </c>
+      <c r="I20">
+        <v>20</v>
+      </c>
+      <c r="J20" t="s">
+        <v>127</v>
+      </c>
+      <c r="K20">
+        <v>10</v>
       </c>
       <c r="Y20" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="Z20">
         <v>10</v>
@@ -1818,34 +1890,34 @@
     </row>
     <row r="21" spans="1:28">
       <c r="A21" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B21">
         <v>9000</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="F21" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G21">
+        <v>1000</v>
+      </c>
+      <c r="H21" t="s">
+        <v>74</v>
+      </c>
+      <c r="I21">
         <v>200</v>
       </c>
-      <c r="H21" t="s">
-        <v>79</v>
-      </c>
-      <c r="I21">
-        <v>100</v>
-      </c>
       <c r="J21" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="K21">
         <v>80</v>
@@ -1854,7 +1926,7 @@
         <v>0.02</v>
       </c>
       <c r="U21" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="V21">
         <v>1.6670000000000001E-2</v>
@@ -1869,43 +1941,43 @@
     </row>
     <row r="22" spans="1:28">
       <c r="A22" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B22">
         <v>9001</v>
       </c>
       <c r="C22" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="F22" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="G22">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="H22" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="I22">
         <v>100</v>
       </c>
       <c r="J22" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="K22">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="L22">
         <v>0.01</v>
       </c>
       <c r="Y22" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="Z22">
         <v>20</v>
@@ -1920,67 +1992,67 @@
     </row>
     <row r="23" spans="1:28">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B23">
         <v>10000</v>
       </c>
       <c r="C23" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="F23" t="s">
-        <v>74</v>
+        <v>122</v>
       </c>
       <c r="G23">
-        <v>400</v>
+        <v>4000</v>
       </c>
       <c r="H23" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="I23">
+        <v>800</v>
+      </c>
+      <c r="J23" t="s">
+        <v>72</v>
+      </c>
+      <c r="K23">
         <v>160</v>
-      </c>
-      <c r="J23" t="s">
-        <v>77</v>
-      </c>
-      <c r="K23">
-        <v>120</v>
       </c>
       <c r="L23">
         <v>0.1</v>
       </c>
       <c r="M23" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="N23">
         <v>15</v>
       </c>
       <c r="O23" t="s">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="P23">
         <v>100</v>
       </c>
       <c r="Q23" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="R23">
         <v>20</v>
       </c>
       <c r="S23" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="T23">
         <v>50</v>
       </c>
       <c r="U23" t="s">
-        <v>93</v>
+        <v>136</v>
       </c>
       <c r="W23">
         <v>720</v>
@@ -1998,31 +2070,43 @@
     </row>
     <row r="24" spans="1:28">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B24">
         <v>10001</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F24" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
       <c r="G24">
         <v>400</v>
       </c>
+      <c r="H24" t="s">
+        <v>128</v>
+      </c>
+      <c r="I24">
+        <v>100</v>
+      </c>
+      <c r="J24" t="s">
+        <v>102</v>
+      </c>
+      <c r="K24">
+        <v>20</v>
+      </c>
       <c r="L24">
         <v>0.05</v>
       </c>
       <c r="Y24" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="Z24">
         <v>1</v>
@@ -2037,61 +2121,61 @@
     </row>
     <row r="25" spans="1:28">
       <c r="A25" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B25">
         <v>11000</v>
       </c>
       <c r="C25" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="F25" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
       <c r="G25">
+        <v>8000</v>
+      </c>
+      <c r="H25" t="s">
+        <v>73</v>
+      </c>
+      <c r="I25">
         <v>400</v>
       </c>
-      <c r="H25" t="s">
-        <v>78</v>
-      </c>
-      <c r="I25">
+      <c r="J25" t="s">
+        <v>72</v>
+      </c>
+      <c r="K25">
         <v>160</v>
-      </c>
-      <c r="J25" t="s">
-        <v>77</v>
-      </c>
-      <c r="K25">
-        <v>120</v>
       </c>
       <c r="L25">
         <v>0.1</v>
       </c>
       <c r="M25" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="N25">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="O25" t="s">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="P25">
         <v>10000</v>
       </c>
       <c r="Q25" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="R25">
         <v>200</v>
       </c>
       <c r="U25" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="W25">
         <v>720</v>
@@ -2109,31 +2193,43 @@
     </row>
     <row r="26" spans="1:28">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B26">
         <v>11001</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F26" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
       <c r="G26">
-        <v>400</v>
+        <v>800</v>
+      </c>
+      <c r="H26" t="s">
+        <v>128</v>
+      </c>
+      <c r="I26">
+        <v>120</v>
+      </c>
+      <c r="J26" t="s">
+        <v>130</v>
+      </c>
+      <c r="K26">
+        <v>20</v>
       </c>
       <c r="L26">
         <v>0.05</v>
       </c>
       <c r="Y26" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="Z26">
         <v>1</v>
@@ -2148,28 +2244,55 @@
     </row>
     <row r="27" spans="1:28">
       <c r="A27" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B27">
         <v>12000</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="F27" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
       <c r="G27">
-        <v>400</v>
+        <v>2000</v>
+      </c>
+      <c r="H27" t="s">
+        <v>129</v>
+      </c>
+      <c r="I27">
+        <v>500</v>
+      </c>
+      <c r="J27" t="s">
+        <v>130</v>
+      </c>
+      <c r="K27">
+        <v>40</v>
       </c>
       <c r="L27">
         <v>0.5</v>
+      </c>
+      <c r="M27" t="s">
+        <v>118</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27" t="s">
+        <v>134</v>
+      </c>
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="U27" t="s">
+        <v>135</v>
       </c>
       <c r="W27">
         <v>1440</v>
@@ -2187,43 +2310,43 @@
     </row>
     <row r="28" spans="1:28">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B28">
         <v>20000</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>132</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F28" t="s">
-        <v>74</v>
+        <v>133</v>
       </c>
       <c r="G28">
         <v>30000</v>
       </c>
       <c r="H28" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="I28">
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="J28" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="K28">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="L28">
         <v>1</v>
       </c>
       <c r="Y28" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="Z28">
         <v>1</v>
@@ -2238,28 +2361,28 @@
     </row>
     <row r="29" spans="1:28">
       <c r="A29" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B29">
-        <v>30000</v>
+        <v>20</v>
       </c>
       <c r="C29" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F29" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G29">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="Y29" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="Z29">
         <v>125</v>
@@ -2274,10 +2397,10 @@
     </row>
     <row r="30" spans="1:28">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C30" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G30">
         <v>4</v>

</xml_diff>